<commit_message>
Best Score Yet: 0.77990
</commit_message>
<xml_diff>
--- a/Titanic/train.xlsx
+++ b/Titanic/train.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="train" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -4543,10 +4543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N895"/>
+  <dimension ref="A1:O895"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A854" workbookViewId="0">
-      <selection activeCell="P890" sqref="P890"/>
+      <selection activeCell="O894" sqref="O894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42461,7 +42461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="881" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="881" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A881">
         <v>880</v>
       </c>
@@ -42507,7 +42507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="882" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="882" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A882">
         <v>881</v>
       </c>
@@ -42550,7 +42550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="883" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="883" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A883">
         <v>882</v>
       </c>
@@ -42593,7 +42593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="884" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="884" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A884">
         <v>883</v>
       </c>
@@ -42636,7 +42636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="885" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="885" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A885">
         <v>884</v>
       </c>
@@ -42679,7 +42679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="886" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="886" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A886">
         <v>885</v>
       </c>
@@ -42722,7 +42722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="887" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="887" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A887">
         <v>886</v>
       </c>
@@ -42765,7 +42765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="888" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="888" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A888">
         <v>887</v>
       </c>
@@ -42808,7 +42808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="889" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="889" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A889">
         <v>888</v>
       </c>
@@ -42854,7 +42854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="890" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="890" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A890">
         <v>889</v>
       </c>
@@ -42894,7 +42894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="891" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="891" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A891">
         <v>890</v>
       </c>
@@ -42940,7 +42940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="892" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="892" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A892">
         <v>891</v>
       </c>
@@ -42983,7 +42983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="893" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="893" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M893" t="s">
         <v>1225</v>
       </c>
@@ -42992,21 +42992,25 @@
         <v>701</v>
       </c>
     </row>
-    <row r="894" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="894" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M894" t="s">
         <v>1224</v>
       </c>
       <c r="N894">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="895" spans="1:14" x14ac:dyDescent="0.3">
+        <v>891</v>
+      </c>
+      <c r="O894">
+        <f>N894-N893</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="895" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M895" t="s">
         <v>1226</v>
       </c>
       <c r="N895" s="1">
         <f>N893/N894</f>
-        <v>0.78764044943820222</v>
+        <v>0.78675645342312006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>